<commit_message>
Code Change in Cell merge.
</commit_message>
<xml_diff>
--- a/JDA_v3/src/test/java/testData/DB.xlsx
+++ b/JDA_v3/src/test/java/testData/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NRavichandran\git\Supersession\JDA_v3\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FED6703-568A-402F-A91F-918DFCD7CFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FC0024-D0F0-425D-BA79-2B62E454056B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,9 +345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -366,7 +364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB25AC7-8DFD-471A-BA8F-A47DEAE78540}">
   <dimension ref="B1:I1"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>